<commit_message>
0 Signed-off-by: 2818724775 <2818724775@qq.com>
</commit_message>
<xml_diff>
--- a/doc/小组log日志/201708044122sms (1).xlsx
+++ b/doc/小组log日志/201708044122sms (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9347" activeTab="1"/>
+    <workbookView windowWidth="12515" windowHeight="9647" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="娄梦月" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>日期时间</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>简单了解web层</t>
+  </si>
+  <si>
+    <t>2019/5/31 18:00-20:00</t>
+  </si>
+  <si>
+    <t>简单项目框架</t>
+  </si>
+  <si>
+    <t>2019/6/11 22:00-24:00</t>
+  </si>
+  <si>
+    <t>提交文档</t>
   </si>
   <si>
     <t>2019/4/15 8:30--10:30</t>
@@ -356,8 +368,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -365,14 +377,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,6 +389,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -405,16 +425,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,20 +463,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -482,15 +488,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -521,18 +533,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -545,163 +707,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,6 +724,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -739,13 +762,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,21 +824,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -820,10 +832,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -832,19 +844,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -853,112 +865,112 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1346,10 +1358,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90740740740741" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1513,6 +1525,22 @@
       </c>
       <c r="B20" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1554,10 +1582,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1602,71 +1630,71 @@
         <v>43561</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1745,66 +1773,66 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1846,18 +1874,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1899,87 +1927,87 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>